<commit_message>
Reorganise API slightly. Test xlsx files resaved using Excel.
</commit_message>
<xml_diff>
--- a/tests/unit/reportFinalization/mock_data/bad_mojaloop_identifier_column.xlsx
+++ b/tests/unit/reportFinalization/mock_data/bad_mojaloop_identifier_column.xlsx
@@ -1,77 +1,104 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
-  <workbookPr date1904="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulmakin/Dropbox/Trouver/Projects/ModusBox/Settlement Test Cases/26:11/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9FD95B3A-FC33-6748-AD1E-1F581557CA82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" windowWidth="9600" windowHeight="8720"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25440" windowHeight="12780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Oct 2021" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">#REF!</definedName>
     <definedName name="_xlnm.Sheet_Title" localSheetId="0">"Oct 2021"</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">#REF!</definedName>
   </definedNames>
-  <calcPr calcMode="auto" iterate="1" iterateCount="100" iterateDelta="0.001"/>
-  <webPublishing allowPng="1" css="0" codePage="1252"/>
+  <calcPr calcId="0" iterate="1"/>
+  <webPublishing css="0" allowPng="1" codePage="1252"/>
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>tc={F97A32E5-197D-F049-8C25-4568C8CD1A60}</author>
-  </authors>
-  <commentList>
-    <comment ref="A7" authorId="0">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    participant_id account_id participant_name</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+  <si>
+    <t>Settlement ID</t>
+  </si>
+  <si>
+    <t>Settlement Completed Date</t>
+  </si>
+  <si>
+    <t>Settlement Completed Time</t>
+  </si>
+  <si>
+    <t>Timezone</t>
+  </si>
+  <si>
+    <t>MMT</t>
+  </si>
+  <si>
+    <t>Participant (WynePay Identifier)</t>
+  </si>
+  <si>
+    <t>Participant (CB Bank Identifier)</t>
+  </si>
+  <si>
+    <t>Balance</t>
+  </si>
+  <si>
+    <t>Settlement Transfer</t>
+  </si>
+  <si>
+    <t>11 21 mmdokdollar</t>
+  </si>
+  <si>
+    <t>Internet Wallet Myanmar Limited
+0086 1005 0000 7617</t>
+  </si>
+  <si>
+    <t>1 19 visionfund</t>
+  </si>
+  <si>
+    <t>Vision Fund Myanmar Co., Ltd
+0086 1005 0003 5351</t>
+  </si>
+  <si>
+    <t>3 hana 25</t>
+  </si>
+  <si>
+    <t>Hana Microfinance Limited
+0086 1005 0003 5335</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)" numFmtId="100"/>
-    <numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" numFmtId="101"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="3">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <u val="none"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Sans"/>
-      <vertAlign val="baseline"/>
-      <sz val="10"/>
-      <strike val="0"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <u val="none"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <vertAlign val="baseline"/>
-      <sz val="11"/>
-      <strike val="0"/>
     </font>
     <font>
-      <b val="1"/>
-      <i val="0"/>
-      <u val="none"/>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <vertAlign val="baseline"/>
-      <sz val="11"/>
-      <strike val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -83,126 +110,453 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="0" diagonalDown="0">
-      <left style="none">
-        <color rgb="FFC7C7C7"/>
-      </left>
-      <right style="none">
-        <color rgb="FFC7C7C7"/>
-      </right>
-      <top style="none">
-        <color rgb="FFC7C7C7"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FFC7C7C7"/>
-      </bottom>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-      <protection locked="1" hidden="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="13">
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-      <protection locked="1" hidden="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-      <protection locked="1" hidden="0"/>
+    <xf numFmtId="15" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="right" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-      <protection locked="1" hidden="0"/>
+    <xf numFmtId="15" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="18" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="0" numFmtId="15" xfId="0">
-      <alignment horizontal="right" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-      <protection locked="1" hidden="0"/>
+    <xf numFmtId="18" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="15" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="0" numFmtId="15" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-      <protection locked="1" hidden="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="0" numFmtId="18" xfId="0">
-      <alignment horizontal="right" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-      <protection locked="1" hidden="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="0" numFmtId="18" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-      <protection locked="1" hidden="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-      <protection locked="1" hidden="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="2" fillId="0" borderId="0" numFmtId="15" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-      <protection locked="1" hidden="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="top" wrapText="1" shrinkToFit="0" textRotation="0" indent="0"/>
-      <protection locked="1" hidden="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="1" shrinkToFit="0" textRotation="0" indent="0"/>
-      <protection locked="1" hidden="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="0" numFmtId="100" xfId="0">
-      <alignment horizontal="general" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-      <protection locked="1" hidden="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="0" numFmtId="101" xfId="0">
-      <alignment horizontal="general" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-      <protection locked="1" hidden="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>774700</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1026" name="#_x0000_t201" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C29F5C1B-E942-3F44-90BD-A5B1E08CEDE9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:gnmx="http://www.gnumeric.org/ext/spreadsheetml">
-  <sheetPr>
-    <pageSetUpPr fitToPage="0"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AY9"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" style="1" width="31.5" customWidth="1"/>
-    <col min="3" max="3" style="1" width="12.83203125" customWidth="1"/>
-    <col min="4" max="4" style="1" width="18.33203125" customWidth="1"/>
-    <col min="5" max="5" style="1" width="12.83203125" customWidth="1"/>
-    <col min="6" max="6" style="1" width="18.33203125" customWidth="1"/>
-    <col min="7" max="7" style="1" width="12.83203125" customWidth="1"/>
-    <col min="8" max="8" style="1" width="18.33203125" customWidth="1"/>
-    <col min="9" max="9" style="1" width="12.83203125" customWidth="1"/>
-    <col min="10" max="10" style="1" width="18.33203125" customWidth="1"/>
-    <col min="11" max="51" style="1" width="12.83203125" customWidth="1"/>
-    <col min="52" max="16384" style="1" width="9.142307692307693"/>
+    <col min="1" max="2" width="31.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="18.33203125" style="1" customWidth="1"/>
+    <col min="11" max="51" width="12.83203125" style="1" customWidth="1"/>
+    <col min="52" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:51">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Settlement ID</t>
-        </is>
+      <c r="A1" t="s">
+        <v>0</v>
       </c>
       <c r="B1" s="2">
         <v>13</v>
       </c>
-      <c r="C1" s="0"/>
+      <c r="C1"/>
     </row>
     <row r="2" spans="1:51">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Settlement Completed Date</t>
-        </is>
+      <c r="A2" t="s">
+        <v>1</v>
       </c>
       <c r="B2" s="3">
         <v>44511</v>
@@ -257,10 +611,8 @@
       <c r="AY2" s="4"/>
     </row>
     <row r="3" spans="1:51">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Settlement Completed Time</t>
-        </is>
+      <c r="A3" t="s">
+        <v>2</v>
       </c>
       <c r="B3" s="5">
         <v>0.45833333333333331</v>
@@ -315,15 +667,11 @@
       <c r="AY3" s="6"/>
     </row>
     <row r="4" spans="1:51">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Timezone</t>
-        </is>
-      </c>
-      <c r="B4" s="5" t="inlineStr">
-        <is>
-          <t>MMT</t>
-        </is>
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>4</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -426,25 +774,17 @@
       <c r="AY5" s="4"/>
     </row>
     <row r="6" spans="1:51">
-      <c r="A6" s="7" t="inlineStr">
-        <is>
-          <t>Participant (WynePay Identifier)</t>
-        </is>
-      </c>
-      <c r="B6" s="7" t="inlineStr">
-        <is>
-          <t>Participant (CB Bank Identifier)</t>
-        </is>
-      </c>
-      <c r="C6" s="8" t="inlineStr">
-        <is>
-          <t>Balance</t>
-        </is>
-      </c>
-      <c r="D6" s="8" t="inlineStr">
-        <is>
-          <t>Settlement Transfer</t>
-        </is>
+      <c r="A6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
@@ -495,16 +835,11 @@
       <c r="AY6" s="8"/>
     </row>
     <row r="7" spans="1:51" ht="32">
-      <c r="A7" s="9" t="inlineStr">
-        <is>
-          <t>11 21 mmdokdollar</t>
-        </is>
-      </c>
-      <c r="B7" s="10" t="inlineStr">
-        <is>
-          <t>Internet Wallet Myanmar Limited
-0086 1005 0000 7617</t>
-        </is>
+      <c r="A7" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="C7" s="11">
         <v>1501000</v>
@@ -561,16 +896,11 @@
       <c r="AY7" s="12"/>
     </row>
     <row r="8" spans="1:51" ht="32">
-      <c r="A8" s="9" t="inlineStr">
-        <is>
-          <t>1 19 visionfund</t>
-        </is>
-      </c>
-      <c r="B8" s="10" t="inlineStr">
-        <is>
-          <t>Vision Fund Myanmar Co., Ltd
-0086 1005 0003 5351</t>
-        </is>
+      <c r="A8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="C8" s="11">
         <v>2200</v>
@@ -627,16 +957,11 @@
       <c r="AY8" s="12"/>
     </row>
     <row r="9" spans="1:51" ht="32">
-      <c r="A9" s="9" t="inlineStr">
-        <is>
-          <t>3 hana 25</t>
-        </is>
-      </c>
-      <c r="B9" s="10" t="inlineStr">
-        <is>
-          <t>Hana Microfinance Limited
-0086 1005 0003 5335</t>
-        </is>
+      <c r="A9" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>14</v>
       </c>
       <c r="C9" s="11">
         <v>2200</v>
@@ -694,13 +1019,8 @@
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
-  <printOptions/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup blackAndWhite="0" cellComments="asDisplayed" draft="0" errors="displayed" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0"/>
-  <headerFooter>
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" cellComments="asDisplayed"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>